<commit_message>
plan for  13 Aug
</commit_message>
<xml_diff>
--- a/DEVASC_Study_Tracker.xlsx
+++ b/DEVASC_Study_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoshiyar.digari/Downloads/devNetstudytracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C9E5CC-36F3-9742-8A84-C7DAA0C866DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9DE688-AFA5-5544-BC59-953A997CF9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1000" windowWidth="34200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
   <si>
     <t>Week</t>
   </si>
@@ -98,6 +98,9 @@
     <t>common design patterns</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>Linux bash</t>
   </si>
   <si>
@@ -108,6 +111,12 @@
   </si>
   <si>
     <t>revise do I know</t>
+  </si>
+  <si>
+    <t>Introduction to Python</t>
+  </si>
+  <si>
+    <t>read through and make notes for whole chapter</t>
   </si>
 </sst>
 </file>
@@ -451,7 +460,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -548,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>0.5</v>
@@ -568,7 +577,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -588,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>0.2</v>
@@ -608,7 +617,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>0.2</v>
@@ -625,7 +634,16 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
working code on sep2
</commit_message>
<xml_diff>
--- a/DEVASC_Study_Tracker.xlsx
+++ b/DEVASC_Study_Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoshiyar.digari/Downloads/devNetstudytracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9DE688-AFA5-5544-BC59-953A997CF9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6697E409-41B0-DA42-8D02-852705DCC285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1000" windowWidth="34200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
   <si>
     <t>Week</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>read through and make notes for whole chapter</t>
+  </si>
+  <si>
+    <t>Pyhton Functions , classes and modules</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -642,8 +645,11 @@
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -651,7 +657,13 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>1.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>